<commit_message>
commit actualizacion 25-08-2023 luis santamaria
</commit_message>
<xml_diff>
--- a/dags/files_pami/Instalada.xlsx
+++ b/dags/files_pami/Instalada.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clinicossasips-my.sharepoint.com/personal/maristizabal_clinicos_com_co/Documents/GESTIÓN DE TABLEROS/ACTUALIZACION PAMI Y CARTAGENA/INSTALADA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clinicos\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="302" documentId="8_{31ADE914-9DE5-4511-AB20-152EDF16DC84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{295DE499-903D-4DD7-B0A6-098FE05AC009}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392EDD39-D3BB-4353-A5AE-3A680DB403B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{3655D678-912F-4640-A6FF-27DCF24D6CD0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="7">
   <si>
     <t>Sede</t>
   </si>
@@ -53,85 +53,10 @@
     <t>Bulevar</t>
   </si>
   <si>
-    <t>MEDICINA GENERAL</t>
-  </si>
-  <si>
-    <t>PEDIATRÍA</t>
-  </si>
-  <si>
-    <t>MEDICINA INTERNA</t>
-  </si>
-  <si>
-    <t>DERMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>GERIATRÍA</t>
-  </si>
-  <si>
-    <t>CARDIOLOGÍA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENDOCRINOLOGÍA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FISIATRÍA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GINECOLOGÍA </t>
-  </si>
-  <si>
     <t xml:space="preserve">ECOCARDIOGRAMA </t>
   </si>
   <si>
     <t>ECOGRAFÍA</t>
-  </si>
-  <si>
-    <t>NUTRICIÓN</t>
-  </si>
-  <si>
-    <t>PSICOLOGÍA</t>
-  </si>
-  <si>
-    <t>TRABAJO SOCIAL</t>
-  </si>
-  <si>
-    <t>TERAPIA OCUPACIONAL</t>
-  </si>
-  <si>
-    <t>TERAPIA RESPIRATORIA</t>
-  </si>
-  <si>
-    <t>San Martin</t>
-  </si>
-  <si>
-    <t>PSIQUIATRÍA</t>
-  </si>
-  <si>
-    <t>Cartagena</t>
-  </si>
-  <si>
-    <t>TERAPIA DE LENGUAJE</t>
-  </si>
-  <si>
-    <t>TERAPIA FÍSICA 1RA VEZ</t>
-  </si>
-  <si>
-    <t>PROCEDIMIENTOS DERMATOLÓGICOS</t>
-  </si>
-  <si>
-    <t>MEDICINA DEL DEPORTE</t>
-  </si>
-  <si>
-    <t>NEUROLOGÍA</t>
-  </si>
-  <si>
-    <t>REUMATOLOGÍA</t>
-  </si>
-  <si>
-    <t>PSIQUIATRÍA INFANTIL</t>
-  </si>
-  <si>
-    <t>TERAPIA FÍSICA SESIONES</t>
   </si>
 </sst>
 </file>
@@ -285,8 +210,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4EB043F7-73AA-4204-82B3-9452EAF3FC9D}" name="Tabla2" displayName="Tabla2" ref="A1:D41" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
-  <autoFilter ref="A1:D41" xr:uid="{4EB043F7-73AA-4204-82B3-9452EAF3FC9D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4EB043F7-73AA-4204-82B3-9452EAF3FC9D}" name="Tabla2" displayName="Tabla2" ref="A1:D15" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
+  <autoFilter ref="A1:D15" xr:uid="{4EB043F7-73AA-4204-82B3-9452EAF3FC9D}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{97C6BDF9-67D2-4EF7-A093-17EE8919158D}" name="Sede"/>
     <tableColumn id="2" xr3:uid="{AEBA6ACF-1126-417E-9C76-C72E8AAEAE7D}" name="Servicio"/>
@@ -594,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DC2D88A-CC9F-4EB7-98D7-86D94DC56E4E}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +558,7 @@
         <v>45108</v>
       </c>
       <c r="D2">
-        <v>516</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -641,13 +566,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
-        <v>45108</v>
+        <v>45078</v>
       </c>
       <c r="D3">
-        <v>288</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -655,13 +580,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
-        <v>45108</v>
+        <v>45047</v>
       </c>
       <c r="D4">
-        <v>360</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -669,13 +594,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1">
-        <v>45108</v>
+        <v>45017</v>
       </c>
       <c r="D5">
-        <v>225</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -683,13 +608,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1">
-        <v>45108</v>
+        <v>44986</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -697,13 +622,13 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1">
-        <v>45108</v>
+        <v>44958</v>
       </c>
       <c r="D7">
-        <v>24</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -711,13 +636,13 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1">
-        <v>45108</v>
+        <v>44927</v>
       </c>
       <c r="D8">
-        <v>180</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -725,13 +650,13 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1">
         <v>45108</v>
       </c>
       <c r="D9">
-        <v>80</v>
+        <v>300</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -739,13 +664,13 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C10" s="1">
-        <v>45108</v>
+        <v>45078</v>
       </c>
       <c r="D10">
-        <v>72</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -753,13 +678,13 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C11" s="1">
-        <v>45108</v>
+        <v>45047</v>
       </c>
       <c r="D11">
-        <v>216</v>
+        <v>300</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -767,13 +692,13 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C12" s="1">
-        <v>45108</v>
+        <v>45017</v>
       </c>
       <c r="D12">
-        <v>151</v>
+        <v>300</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -781,10 +706,10 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1">
-        <v>45108</v>
+        <v>44986</v>
       </c>
       <c r="D13">
         <v>300</v>
@@ -795,13 +720,13 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C14" s="1">
-        <v>45108</v>
+        <v>44958</v>
       </c>
       <c r="D14">
-        <v>328</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -809,377 +734,13 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C15" s="1">
-        <v>45108</v>
+        <v>44927</v>
       </c>
       <c r="D15">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="1">
-        <v>45108</v>
-      </c>
-      <c r="D16">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="1">
-        <v>45108</v>
-      </c>
-      <c r="D17">
-        <v>2056</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="1">
-        <v>45108</v>
-      </c>
-      <c r="D18">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="1">
-        <v>45108</v>
-      </c>
-      <c r="D19">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="1">
-        <v>45108</v>
-      </c>
-      <c r="D20">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="1">
-        <v>45108</v>
-      </c>
-      <c r="D21">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="1">
-        <v>45108</v>
-      </c>
-      <c r="D22">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="1">
-        <v>45108</v>
-      </c>
-      <c r="D23">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="1">
-        <v>45108</v>
-      </c>
-      <c r="D24">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="1">
-        <v>45108</v>
-      </c>
-      <c r="D25">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="1">
-        <v>45108</v>
-      </c>
-      <c r="D26">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="1">
-        <v>45108</v>
-      </c>
-      <c r="D27">
         <v>300</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="1">
-        <v>45108</v>
-      </c>
-      <c r="D28">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" t="s">
-        <v>20</v>
-      </c>
-      <c r="C29" s="1">
-        <v>45108</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" t="s">
-        <v>31</v>
-      </c>
-      <c r="C30" s="1">
-        <v>45108</v>
-      </c>
-      <c r="D30">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>21</v>
-      </c>
-      <c r="B31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="1">
-        <v>45108</v>
-      </c>
-      <c r="D31">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>21</v>
-      </c>
-      <c r="B32" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" s="1">
-        <v>45108</v>
-      </c>
-      <c r="D32">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>23</v>
-      </c>
-      <c r="B33" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="1">
-        <v>45108</v>
-      </c>
-      <c r="D33">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" t="s">
-        <v>31</v>
-      </c>
-      <c r="C34" s="1">
-        <v>45108</v>
-      </c>
-      <c r="D34">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>23</v>
-      </c>
-      <c r="B35" t="s">
-        <v>25</v>
-      </c>
-      <c r="C35" s="1">
-        <v>45108</v>
-      </c>
-      <c r="D35">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>23</v>
-      </c>
-      <c r="B36" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="1">
-        <v>45108</v>
-      </c>
-      <c r="D36">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37" t="s">
-        <v>28</v>
-      </c>
-      <c r="C37" s="1">
-        <v>45108</v>
-      </c>
-      <c r="D37">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>23</v>
-      </c>
-      <c r="B38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" s="1">
-        <v>45108</v>
-      </c>
-      <c r="D38">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>23</v>
-      </c>
-      <c r="B39" t="s">
-        <v>12</v>
-      </c>
-      <c r="C39" s="1">
-        <v>45108</v>
-      </c>
-      <c r="D39">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>23</v>
-      </c>
-      <c r="B40" t="s">
-        <v>29</v>
-      </c>
-      <c r="C40" s="1">
-        <v>45108</v>
-      </c>
-      <c r="D40">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>23</v>
-      </c>
-      <c r="B41" t="s">
-        <v>30</v>
-      </c>
-      <c r="C41" s="1">
-        <v>45108</v>
-      </c>
-      <c r="D41">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1371,9 +932,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02C080E4-4A92-4583-93C5-A87FF940F702}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3ED1D98A-FAD0-4836-9ABF-0F5D0769719F}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6E75A56-E4D9-4A8A-97FA-EE13411B96B1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC25D276-6DB4-4C97-A8E5-7D22F5D0B78A}"/>
 </file>
</xml_diff>